<commit_message>
Max range results for unit 235  #1
</commit_message>
<xml_diff>
--- a/scripts/maxRange/Results.xlsx
+++ b/scripts/maxRange/Results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Plot all scenes with ROI marked.</t>
+  </si>
+  <si>
+    <t>Look at the effect of the LPF Avihai pointed out</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,6 +1016,9 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>